<commit_message>
Subida de todos los archivos y últimos cambios
</commit_message>
<xml_diff>
--- a/static/temp/resultado_cruce.xlsx
+++ b/static/temp/resultado_cruce.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,201 @@
       <c r="K1" s="1" t="inlineStr">
         <is>
           <t>_merge</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Mesa y Lopez</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Z010100004</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CAMEL ACTIVA 10x20 Udes.</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>8416500103257</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-05-23 14:13:39</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>left_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Mesa y Lopez</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Z010100003</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CAMEL ACTIVA DOBLE 20x10 Udes.</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>8416500103325</v>
+      </c>
+      <c r="F3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-05-23 14:19:20</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>left_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Mesa y Lopez</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Z010100003</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CAMEL ACTIVA DOBLE 20x10 Udes.</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>8416500103325</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-05-23 14:13:39</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>left_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Mesa y Lopez</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Z010100020</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CAMEL RYO LEGEND 10X30 Grms.</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>8416500021797</v>
+      </c>
+      <c r="F5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-05-23 14:13:39</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>left_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Mesa y Lopez</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Z010200000</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>WINSTON CLAS.BOX CT 10x20 Ude.</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>8416500140948</v>
+      </c>
+      <c r="F6" t="n">
+        <v>20</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-05-23 14:13:39</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>left_only</t>
         </is>
       </c>
     </row>
@@ -503,7 +698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -777,22 +972,22 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>CAMEL FILTERS SOFT 10x20 Udes.</t>
+          <t>CAMEL BLUE CARTON 10x20 Ud.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
-        <v>2011000002</v>
+        <v>2011000001</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>720 20156</t>
+          <t>720 12103</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -806,22 +1001,22 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>CAMEL RYO y LEGEND 10x30Gr</t>
+          <t>CAMEL FILTERS SOFT 10x20 Udes.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
-        <v>2011000006</v>
+        <v>2011000002</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>720 22336</t>
+          <t>720 20156</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -835,22 +1030,22 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CAMEL Yellow 10x23 Udes.</t>
+          <t>CAMEL RYO y LEGEND 10x30Gr</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
-        <v>2011000005</v>
+        <v>2011000006</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>720 12114</t>
+          <t>720 22336</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -864,22 +1059,22 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CORONAS DE LA TIERRA 20x5</t>
+          <t>CAMEL Yellow 10x23 Udes.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
-        <v>2011001008</v>
+        <v>2011000005</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>720 20794</t>
+          <t>720 12114</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -900,7 +1095,7 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
-        <v>2011001009</v>
+        <v>2011001008</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -922,22 +1117,22 @@
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CORONAS NEGRO 10x20</t>
+          <t>CORONAS DE LA TIERRA 20x5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
-        <v>2011001010</v>
+        <v>2011001009</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>720 20788</t>
+          <t>720 20794</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -958,7 +1153,7 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
-        <v>2011001011</v>
+        <v>2011001010</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -966,7 +1161,7 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -980,22 +1175,22 @@
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>CORONAS SILVER 10x20</t>
+          <t>CORONAS NEGRO 10x20</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
-        <v>2011001012</v>
+        <v>2011001011</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>720 20974</t>
+          <t>720 20788</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1016,7 +1211,7 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
-        <v>2011001013</v>
+        <v>2011001012</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1038,22 +1233,22 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>DIP.PLOOM DEVICE AVANCE BLACK</t>
+          <t>CORONAS SILVER 10x20</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
-        <v>2015000033</v>
+        <v>2011001013</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>720 2015000053</t>
+          <t>720 20974</t>
         </is>
       </c>
       <c r="J18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -1067,18 +1262,18 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>DIP.PLOOM DEVICE AVANCE NAVY P</t>
+          <t>DIP.PLOOM DEVICE AVANCE BLACK</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
-        <v>2015000031</v>
+        <v>2015000033</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>720 2015000051</t>
+          <t>720 2015000053</t>
         </is>
       </c>
       <c r="J19" t="n">
@@ -1096,18 +1291,18 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>DIP.PLOOM DEVICE AVANCE SILVER</t>
+          <t>DIP.PLOOM DEVICE AVANCE NAVY P</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
-        <v>2015000032</v>
+        <v>2015000031</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>720 2015000052</t>
+          <t>720 2015000051</t>
         </is>
       </c>
       <c r="J20" t="n">
@@ -1125,22 +1320,22 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>MAYFAIR KS 10x20</t>
+          <t>DIP.PLOOM DEVICE AVANCE SILVER</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>2015000003</v>
+        <v>2015000032</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>720 12270</t>
+          <t>720 2015000052</t>
         </is>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -1154,18 +1349,18 @@
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>MAYFAIR SKY BLUE 10x20 Ud.</t>
+          <t>MAYFAIR KS 10x20</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
-        <v>2019000021</v>
+        <v>2015000003</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>720 201900001</t>
+          <t>720 12270</t>
         </is>
       </c>
       <c r="J22" t="n">
@@ -1183,22 +1378,22 @@
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>PLOOM CAMEL AMBER CRT.10X20</t>
+          <t>MAYFAIR SKY BLUE 10x20 Ud.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
-        <v>2015000010</v>
+        <v>2019000021</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>720 2015000005</t>
+          <t>720 201900001</t>
         </is>
       </c>
       <c r="J23" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -1212,22 +1407,22 @@
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>PLOOM CAMEL AQUAMAR.CART.10x20</t>
+          <t>PLOOM CAMEL AMBER CRT.10X20</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
-        <v>2015000002</v>
+        <v>2015000010</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>720 13801</t>
+          <t>720 2015000005</t>
         </is>
       </c>
       <c r="J24" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -1241,22 +1436,22 @@
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>PLOOM CAMEL BRONZE CART.10x20</t>
+          <t>PLOOM CAMEL AQUAMAR.CART.10x20</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
-        <v>2015000007</v>
+        <v>2015000002</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>720 2015000002</t>
+          <t>720 13801</t>
         </is>
       </c>
       <c r="J25" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -1270,22 +1465,22 @@
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>PLOOM CAMEL BURGUNDY CRT.10X20</t>
+          <t>PLOOM CAMEL BRONZE CART.10x20</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
-        <v>2015000009</v>
+        <v>2015000007</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>720 2015000004</t>
+          <t>720 2015000002</t>
         </is>
       </c>
       <c r="J26" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
@@ -1299,22 +1494,22 @@
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>PLOOM CAMEL GOLD CART.10X20</t>
+          <t>PLOOM CAMEL BURGUNDY CRT.10X20</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="n">
-        <v>2015000008</v>
+        <v>2015000009</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>720 13803</t>
+          <t>720 2015000004</t>
         </is>
       </c>
       <c r="J27" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
@@ -1328,22 +1523,22 @@
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>PLOOM CAMEL TEAL CARTON 10x20</t>
+          <t>PLOOM CAMEL GOLD CART.10X20</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>2015000001</v>
+        <v>2015000008</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>720 2015000000</t>
+          <t>720 13803</t>
         </is>
       </c>
       <c r="J28" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
@@ -1357,22 +1552,22 @@
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>RYO AMER.SPIRIT ORANG.5x30Grs</t>
+          <t>PLOOM CAMEL TEAL CARTON 10x20</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="n">
-        <v>2013000001</v>
+        <v>2015000001</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>720 22333</t>
+          <t>720 2015000000</t>
         </is>
       </c>
       <c r="J29" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -1386,22 +1581,22 @@
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>RYO AMER.SPIRIT YELLOW 5x30Grs</t>
+          <t>RYO AMER.SPIRIT ORANG.5x30Grs</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="n">
-        <v>2013000002</v>
+        <v>2013000001</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>720 22331</t>
+          <t>720 22333</t>
         </is>
       </c>
       <c r="J30" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
@@ -1415,22 +1610,22 @@
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>SILK CUT PURPLE 10x20 Ud.</t>
+          <t>RYO AMER.SPIRIT YELLOW 5x30Grs</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
-        <v>2015000005</v>
+        <v>2013000002</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>720 12252</t>
+          <t>720 22331</t>
         </is>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
@@ -1444,18 +1639,18 @@
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>SILK CUT WHITE 10x20</t>
+          <t>SILK CUT PURPLE 10x20 Ud.</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
-        <v>2015000004</v>
+        <v>2015000005</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>720 20744</t>
+          <t>720 12252</t>
         </is>
       </c>
       <c r="J32" t="n">
@@ -1473,18 +1668,18 @@
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>STERLING DUAL 10x20 Ud.</t>
+          <t>SILK CUT WHITE 10x20</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
-        <v>2019000023</v>
+        <v>2015000004</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>720 12411</t>
+          <t>720 20744</t>
         </is>
       </c>
       <c r="J33" t="n">
@@ -1502,18 +1697,18 @@
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>STERLING KS 10x20 Ud.</t>
+          <t>STERLING DUAL 10x20 Ud.</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
-        <v>2019000022</v>
+        <v>2019000023</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>720 201900020</t>
+          <t>720 12411</t>
         </is>
       </c>
       <c r="J34" t="n">
@@ -1531,22 +1726,22 @@
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>STERLING RYO 10x50g</t>
+          <t>STERLING KS 10x20 Ud.</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
-        <v>2019000025</v>
+        <v>2019000022</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>720 201900030</t>
+          <t>720 201900020</t>
         </is>
       </c>
       <c r="J35" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
@@ -1560,22 +1755,22 @@
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>STERLING SUPERKING 10X20</t>
+          <t>STERLING RYO 10x50g</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
-        <v>2019000024</v>
+        <v>2019000025</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>720 201900022</t>
+          <t>720 201900030</t>
         </is>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
@@ -1589,22 +1784,22 @@
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>WINSTON BLUE CARTON 10x20</t>
+          <t>STERLING SUPERKING 10X20</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="n">
-        <v>2011001002</v>
+        <v>2019000024</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>720 12212</t>
+          <t>720 201900022</t>
         </is>
       </c>
       <c r="J37" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
@@ -1618,22 +1813,22 @@
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>WINSTON CLAS.BOX CT 10x20</t>
+          <t>WINSTON BLUE CARTON 10x20</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
-        <v>2011001000</v>
+        <v>2011001002</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>720 12200</t>
+          <t>720 12212</t>
         </is>
       </c>
       <c r="J38" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -1647,22 +1842,22 @@
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>WINSTON COMPACT BLUE 10x20</t>
+          <t>WINSTON CLAS.BOX CT 10x20</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="n">
-        <v>2011001005</v>
+        <v>2011001000</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>720 22012</t>
+          <t>720 12200</t>
         </is>
       </c>
       <c r="J39" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
@@ -1676,22 +1871,22 @@
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>WINSTON RED 10x20 Uds.</t>
+          <t>WINSTON COMPACT BLUE 10x20</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="n">
-        <v>2011001007</v>
+        <v>2011001005</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>720 2010200009</t>
+          <t>720 22012</t>
         </is>
       </c>
       <c r="J40" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
@@ -1705,18 +1900,18 @@
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>WINSTON RED 24x8 Uds.</t>
+          <t>WINSTON RED 10x20 Uds.</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
-        <v>2011001006</v>
+        <v>2011001007</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>720 22013</t>
+          <t>720 2010200009</t>
         </is>
       </c>
       <c r="J41" t="n">
@@ -1734,22 +1929,22 @@
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>WINSTON RED BOX 10x20</t>
+          <t>WINSTON RED 24x8 Uds.</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
-        <v>2011001001</v>
+        <v>2011001006</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>720 12211</t>
+          <t>720 22013</t>
         </is>
       </c>
       <c r="J42" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
@@ -1763,22 +1958,22 @@
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr">
         <is>
-          <t>WINSTON RED CARTON 10x20</t>
+          <t>WINSTON RED BOX 10x20</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
-        <v>2011001003</v>
+        <v>2011001001</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>720 12221</t>
+          <t>720 12211</t>
         </is>
       </c>
       <c r="J43" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
@@ -1792,24 +1987,53 @@
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
-          <t>WINSTON RED SOFT 10x20</t>
+          <t>WINSTON RED CARTON 10x20</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
+        <v>2011001003</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>720 12221</t>
+        </is>
+      </c>
+      <c r="J44" t="n">
+        <v>6</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>right_only</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>WINSTON RED SOFT 10x20</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="n">
         <v>2011001004</v>
       </c>
-      <c r="I44" t="inlineStr">
+      <c r="I45" t="inlineStr">
         <is>
           <t>720 12006</t>
         </is>
       </c>
-      <c r="J44" t="n">
+      <c r="J45" t="n">
         <v>3</v>
       </c>
-      <c r="K44" t="inlineStr">
+      <c r="K45" t="inlineStr">
         <is>
           <t>right_only</t>
         </is>
@@ -1826,7 +2050,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1898,42 +2122,44 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4292</v>
+        <v>6</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Mesa y Lopez</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>20101000003</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Z010100000</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CAMEL BLUE CARTON 10x20 Ud.</t>
+          <t>CAMEL FILTERS CARTON 10x20 Ud.</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>8410016804549</v>
+        <v>8416500140962</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-20 15:41:44</t>
+          <t>2025-05-23 14:22:25</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>2011000001</v>
+        <v>2011000000</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>720 12103</t>
+          <t>720 12100</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -1941,55 +2167,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>4291</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Mesa y Lopez</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>20101000002</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CAMEL FILTERS CARTON 10x20 Ud.</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>8410016804556</v>
-      </c>
-      <c r="F3" t="n">
-        <v>10</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-05-20 15:40:53</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>2011000000</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>720 12100</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>17</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>both</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>-7</v>
+        <v>-10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>